<commit_message>
feat：some p0 bug fix
</commit_message>
<xml_diff>
--- a/pet-simulator/Excel/AreaDivide_区域划分表.xlsx
+++ b/pet-simulator/Excel/AreaDivide_区域划分表.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="165">
   <si>
     <t xml:space="preserve">int</t>
   </si>
@@ -612,7 +612,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * \-??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="微软雅黑"/>
@@ -669,6 +669,12 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10.5"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -718,7 +724,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -727,15 +733,15 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -743,7 +749,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -755,7 +761,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -771,6 +781,112 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -778,8 +894,8 @@
   </sheetPr>
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L16" activeCellId="0" sqref="L16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K8" activeCellId="0" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.0859375" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -791,7 +907,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="20.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="22.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="22.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="20.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="25.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="63.02"/>
@@ -1157,7 +1273,9 @@
       <c r="J11" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="K11" s="2"/>
+      <c r="K11" s="9" t="s">
+        <v>54</v>
+      </c>
       <c r="L11" s="2" t="n">
         <v>1000</v>
       </c>
@@ -1941,7 +2059,7 @@
       <c r="E35" s="3" t="n">
         <v>7500000000</v>
       </c>
-      <c r="F35" s="9" t="n">
+      <c r="F35" s="10" t="n">
         <v>65000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat：update six area coin
</commit_message>
<xml_diff>
--- a/pet-simulator/Excel/AreaDivide_区域划分表.xlsx
+++ b/pet-simulator/Excel/AreaDivide_区域划分表.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="161">
   <si>
     <t xml:space="preserve">int</t>
   </si>
@@ -286,6 +286,9 @@
     <t xml:space="preserve">3674D2A0</t>
   </si>
   <si>
+    <t xml:space="preserve">-4771|-40930|4348|-34123|-999|999</t>
+  </si>
+  <si>
     <t xml:space="preserve">海底</t>
   </si>
   <si>
@@ -322,28 +325,13 @@
     <t xml:space="preserve">AreaDivide_Name_10</t>
   </si>
   <si>
-    <t xml:space="preserve">100|-54195|150</t>
+    <t xml:space="preserve">-6021.7|-50088|153.5</t>
   </si>
   <si>
     <t xml:space="preserve">28492BFE</t>
   </si>
   <si>
     <t xml:space="preserve">-4771|-58445|4348|-55900|-999|999</t>
-  </si>
-  <si>
-    <t xml:space="preserve">秘密基地</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AreaDivide_Name_11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1464|-37085|150</t>
-  </si>
-  <si>
-    <t xml:space="preserve">106FD01F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-7300|-39052|-3455|-35407|-999|999</t>
   </si>
   <si>
     <t xml:space="preserve">幻想商店</t>
@@ -892,10 +880,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L35"/>
+  <dimension ref="A1:L1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K8" activeCellId="0" sqref="K8"/>
+      <selection pane="topLeft" activeCell="K13" activeCellId="0" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.0859375" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1274,7 +1262,7 @@
         <v>58</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="L11" s="2" t="n">
         <v>1000</v>
@@ -1285,7 +1273,7 @@
         <v>1008</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>1</v>
@@ -1303,16 +1291,16 @@
         <v>174840</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="L12" s="2" t="n">
         <v>1000</v>
@@ -1323,7 +1311,7 @@
         <v>1009</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C13" s="2" t="n">
         <v>1</v>
@@ -1341,16 +1329,16 @@
         <v>174833</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="L13" s="2" t="n">
         <v>1000</v>
@@ -1361,7 +1349,7 @@
         <v>1010</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C14" s="2" t="n">
         <v>1</v>
@@ -1379,60 +1367,49 @@
         <v>174840</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="n">
-        <v>1011</v>
+        <v>2001</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C15" s="2" t="n">
         <v>1</v>
-      </c>
-      <c r="D15" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E15" s="3" t="n">
-        <v>7500000000</v>
       </c>
       <c r="F15" s="3" t="n">
         <v>50000</v>
       </c>
       <c r="G15" s="2" t="n">
-        <v>174833</v>
+        <v>177826</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="J15" s="2" t="s">
         <v>77</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="L15" s="2" t="n">
-        <v>1000</v>
-      </c>
+      <c r="L15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
-        <v>2001</v>
+        <v>2002</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>79</v>
@@ -1441,10 +1418,10 @@
         <v>1</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>50000</v>
+        <v>20000</v>
       </c>
       <c r="G16" s="2" t="n">
-        <v>177826</v>
+        <v>180217</v>
       </c>
       <c r="H16" s="8" t="s">
         <v>80</v>
@@ -1459,7 +1436,7 @@
     </row>
     <row r="17" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="n">
-        <v>2002</v>
+        <v>2003</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>83</v>
@@ -1467,11 +1444,17 @@
       <c r="C17" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="D17" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E17" s="3" t="n">
+        <v>37500</v>
+      </c>
       <c r="F17" s="3" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="G17" s="2" t="n">
-        <v>180217</v>
+        <v>174840</v>
       </c>
       <c r="H17" s="8" t="s">
         <v>84</v>
@@ -1479,17 +1462,20 @@
       <c r="I17" s="2" t="s">
         <v>85</v>
       </c>
+      <c r="J17" s="2" t="s">
+        <v>86</v>
+      </c>
       <c r="K17" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="n">
-        <v>2003</v>
+        <v>2004</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C18" s="2" t="n">
         <v>1</v>
@@ -1498,34 +1484,34 @@
         <v>3</v>
       </c>
       <c r="E18" s="3" t="n">
-        <v>37500</v>
+        <v>85000</v>
       </c>
       <c r="F18" s="3" t="n">
-        <v>30000</v>
+        <v>25000</v>
       </c>
       <c r="G18" s="2" t="n">
         <v>174840</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="L18" s="2"/>
     </row>
     <row r="19" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="n">
-        <v>2004</v>
+        <v>2005</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C19" s="2" t="n">
         <v>1</v>
@@ -1534,7 +1520,7 @@
         <v>3</v>
       </c>
       <c r="E19" s="3" t="n">
-        <v>85000</v>
+        <v>525000</v>
       </c>
       <c r="F19" s="3" t="n">
         <v>25000</v>
@@ -1543,25 +1529,25 @@
         <v>174840</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="L19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="n">
-        <v>2005</v>
+        <v>2006</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C20" s="2" t="n">
         <v>1</v>
@@ -1570,7 +1556,7 @@
         <v>3</v>
       </c>
       <c r="E20" s="3" t="n">
-        <v>525000</v>
+        <v>3500000</v>
       </c>
       <c r="F20" s="3" t="n">
         <v>25000</v>
@@ -1578,26 +1564,25 @@
       <c r="G20" s="2" t="n">
         <v>174840</v>
       </c>
-      <c r="H20" s="8" t="s">
-        <v>98</v>
+      <c r="H20" s="2" t="s">
+        <v>99</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="L20" s="2"/>
+        <v>102</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="n">
-        <v>2006</v>
+        <v>2007</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C21" s="2" t="n">
         <v>1</v>
@@ -1606,7 +1591,7 @@
         <v>3</v>
       </c>
       <c r="E21" s="3" t="n">
-        <v>3500000</v>
+        <v>18500000</v>
       </c>
       <c r="F21" s="3" t="n">
         <v>25000</v>
@@ -1615,24 +1600,24 @@
         <v>174840</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="n">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C22" s="2" t="n">
         <v>1</v>
@@ -1641,33 +1626,33 @@
         <v>3</v>
       </c>
       <c r="E22" s="3" t="n">
-        <v>18500000</v>
+        <v>66666666</v>
       </c>
       <c r="F22" s="3" t="n">
-        <v>25000</v>
+        <v>30000</v>
       </c>
       <c r="G22" s="2" t="n">
         <v>174840</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C23" s="2" t="n">
         <v>1</v>
@@ -1676,33 +1661,33 @@
         <v>3</v>
       </c>
       <c r="E23" s="3" t="n">
-        <v>66666666</v>
+        <v>150000000</v>
       </c>
       <c r="F23" s="3" t="n">
-        <v>30000</v>
+        <v>35000</v>
       </c>
       <c r="G23" s="2" t="n">
         <v>174840</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="n">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C24" s="2" t="n">
         <v>1</v>
@@ -1711,56 +1696,47 @@
         <v>3</v>
       </c>
       <c r="E24" s="3" t="n">
-        <v>150000000</v>
+        <v>777000000</v>
       </c>
       <c r="F24" s="3" t="n">
-        <v>35000</v>
+        <v>50000</v>
       </c>
       <c r="G24" s="2" t="n">
         <v>174840</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="n">
-        <v>2010</v>
+        <v>3001</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C25" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D25" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="E25" s="3" t="n">
-        <v>777000000</v>
-      </c>
       <c r="F25" s="3" t="n">
-        <v>50000</v>
+        <v>65000</v>
       </c>
       <c r="G25" s="2" t="n">
-        <v>174840</v>
+        <v>177826</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="J25" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K25" s="2" t="s">
@@ -1769,7 +1745,7 @@
     </row>
     <row r="26" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="n">
-        <v>3001</v>
+        <v>3002</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>127</v>
@@ -1778,10 +1754,10 @@
         <v>1</v>
       </c>
       <c r="F26" s="3" t="n">
-        <v>65000</v>
+        <v>30000</v>
       </c>
       <c r="G26" s="2" t="n">
-        <v>177826</v>
+        <v>174840</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>128</v>
@@ -1795,7 +1771,7 @@
     </row>
     <row r="27" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="n">
-        <v>3002</v>
+        <v>3003</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>131</v>
@@ -1803,6 +1779,12 @@
       <c r="C27" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="D27" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="E27" s="3" t="n">
+        <v>50000</v>
+      </c>
       <c r="F27" s="3" t="n">
         <v>30000</v>
       </c>
@@ -1815,16 +1797,19 @@
       <c r="I27" s="2" t="s">
         <v>133</v>
       </c>
+      <c r="J27" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="K27" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="n">
-        <v>3003</v>
+        <v>3004</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C28" s="2" t="n">
         <v>1</v>
@@ -1833,7 +1818,7 @@
         <v>4</v>
       </c>
       <c r="E28" s="3" t="n">
-        <v>50000</v>
+        <v>625000</v>
       </c>
       <c r="F28" s="3" t="n">
         <v>30000</v>
@@ -1842,24 +1827,24 @@
         <v>174840</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="n">
-        <v>3004</v>
+        <v>3005</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C29" s="2" t="n">
         <v>1</v>
@@ -1868,33 +1853,33 @@
         <v>4</v>
       </c>
       <c r="E29" s="3" t="n">
-        <v>625000</v>
+        <v>11500000</v>
       </c>
       <c r="F29" s="3" t="n">
-        <v>30000</v>
+        <v>45000</v>
       </c>
       <c r="G29" s="2" t="n">
         <v>174840</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="n">
-        <v>3005</v>
+        <v>3006</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C30" s="2" t="n">
         <v>1</v>
@@ -1903,33 +1888,33 @@
         <v>4</v>
       </c>
       <c r="E30" s="3" t="n">
-        <v>11500000</v>
+        <v>8250000</v>
       </c>
       <c r="F30" s="3" t="n">
-        <v>45000</v>
+        <v>35000</v>
       </c>
       <c r="G30" s="2" t="n">
         <v>174840</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="n">
-        <v>3006</v>
+        <v>3007</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C31" s="2" t="n">
         <v>1</v>
@@ -1938,33 +1923,33 @@
         <v>4</v>
       </c>
       <c r="E31" s="3" t="n">
-        <v>8250000</v>
+        <v>72500000</v>
       </c>
       <c r="F31" s="3" t="n">
-        <v>35000</v>
+        <v>40000</v>
       </c>
       <c r="G31" s="2" t="n">
         <v>174840</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="n">
-        <v>3007</v>
+        <v>3008</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C32" s="2" t="n">
         <v>1</v>
@@ -1973,33 +1958,30 @@
         <v>4</v>
       </c>
       <c r="E32" s="3" t="n">
-        <v>72500000</v>
+        <v>2500000000</v>
       </c>
       <c r="F32" s="3" t="n">
-        <v>40000</v>
+        <v>65000</v>
       </c>
       <c r="G32" s="2" t="n">
         <v>174840</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="n">
-        <v>3008</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>160</v>
+        <v>3009</v>
       </c>
       <c r="C33" s="2" t="n">
         <v>1</v>
@@ -2008,30 +1990,15 @@
         <v>4</v>
       </c>
       <c r="E33" s="3" t="n">
-        <v>2500000000</v>
+        <v>350000000</v>
       </c>
       <c r="F33" s="3" t="n">
-        <v>65000</v>
-      </c>
-      <c r="G33" s="2" t="n">
-        <v>174840</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="K33" s="2" t="s">
-        <v>164</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="n">
-        <v>3009</v>
+        <v>3010</v>
       </c>
       <c r="C34" s="2" t="n">
         <v>1</v>
@@ -2040,29 +2007,13 @@
         <v>4</v>
       </c>
       <c r="E34" s="3" t="n">
-        <v>350000000</v>
-      </c>
-      <c r="F34" s="3" t="n">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="2" t="n">
-        <v>3010</v>
-      </c>
-      <c r="C35" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D35" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="E35" s="3" t="n">
         <v>7500000000</v>
       </c>
-      <c r="F35" s="10" t="n">
+      <c r="F34" s="10" t="n">
         <v>65000</v>
       </c>
     </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
feat：update coin prefab and area change
</commit_message>
<xml_diff>
--- a/pet-simulator/Excel/AreaDivide_区域划分表.xlsx
+++ b/pet-simulator/Excel/AreaDivide_区域划分表.xlsx
@@ -313,7 +313,7 @@
     <t xml:space="preserve">100|-48094|150</t>
   </si>
   <si>
-    <t xml:space="preserve">250886BE</t>
+    <t xml:space="preserve">21E5ED18</t>
   </si>
   <si>
     <t xml:space="preserve">-4771|-55900|4348|-47640|-999|999</t>
@@ -883,7 +883,7 @@
   <dimension ref="A1:L1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K13" activeCellId="0" sqref="K13"/>
+      <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.0859375" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
feat:update areadivide and droppoint excel
</commit_message>
<xml_diff>
--- a/pet-simulator/Excel/AreaDivide_区域划分表.xlsx
+++ b/pet-simulator/Excel/AreaDivide_区域划分表.xlsx
@@ -882,8 +882,8 @@
   </sheetPr>
   <dimension ref="A1:L1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K9" activeCellId="0" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.0859375" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1432,7 +1432,9 @@
       <c r="K16" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="L16" s="2"/>
+      <c r="L16" s="2" t="n">
+        <v>81000</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="n">

</xml_diff>

<commit_message>
feat:update droppoint and areaworld excel
</commit_message>
<xml_diff>
--- a/pet-simulator/Excel/AreaDivide_区域划分表.xlsx
+++ b/pet-simulator/Excel/AreaDivide_区域划分表.xlsx
@@ -882,8 +882,8 @@
   </sheetPr>
   <dimension ref="A1:L1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K9" activeCellId="0" sqref="K9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E35" activeCellId="0" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.0859375" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
feat:pet 2002 area test
</commit_message>
<xml_diff>
--- a/pet-simulator/Excel/AreaDivide_区域划分表.xlsx
+++ b/pet-simulator/Excel/AreaDivide_区域划分表.xlsx
@@ -355,7 +355,33 @@
     <t xml:space="preserve">-18213|95737|79382</t>
   </si>
   <si>
-    <t xml:space="preserve">-16124.14|-21625.14|97548.13|90734.13|79225.33|80482.33</t>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">'-16124.14|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">97548.13</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">|-21625.14|90734.13|78500.33|80482.33</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">传送门</t>
@@ -600,7 +626,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * \-??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="微软雅黑"/>
@@ -662,6 +688,12 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -883,7 +915,7 @@
   <dimension ref="A1:L1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E35" activeCellId="0" sqref="E35"/>
+      <selection pane="topLeft" activeCell="H36" activeCellId="0" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.0859375" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
feat：update pet world2 wall
</commit_message>
<xml_diff>
--- a/pet-simulator/Excel/AreaDivide_区域划分表.xlsx
+++ b/pet-simulator/Excel/AreaDivide_区域划分表.xlsx
@@ -355,33 +355,7 @@
     <t xml:space="preserve">-18213|95737|79382</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">'-16124.14|</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">97548.13</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">|-21625.14|90734.13|78500.33|80482.33</t>
-    </r>
+    <t xml:space="preserve">-21625.14|90734.13|-16124.14|97548.13|78500.33|80482.33</t>
   </si>
   <si>
     <t xml:space="preserve">传送门</t>
@@ -622,11 +596,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * \-??_ ;_ @_ "/>
+    <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="微软雅黑"/>
@@ -689,12 +664,6 @@
       <family val="0"/>
       <charset val="134"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -744,7 +713,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -781,7 +750,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -914,8 +887,8 @@
   </sheetPr>
   <dimension ref="A1:L1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H36" activeCellId="0" sqref="H36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K21" activeCellId="0" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.0859375" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1076,7 +1049,7 @@
       <c r="I5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="K5" s="9" t="s">
         <v>31</v>
       </c>
       <c r="L5" s="2"/>
@@ -1103,7 +1076,7 @@
       <c r="I6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="K6" s="9" t="s">
         <v>35</v>
       </c>
       <c r="L6" s="2" t="n">
@@ -1141,7 +1114,7 @@
       <c r="J7" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="K7" s="9" t="s">
         <v>40</v>
       </c>
       <c r="L7" s="2" t="n">
@@ -1179,7 +1152,7 @@
       <c r="J8" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="K8" s="9" t="s">
         <v>45</v>
       </c>
       <c r="L8" s="2" t="n">
@@ -1217,7 +1190,7 @@
       <c r="J9" s="2" t="n">
         <v>32519069</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="K9" s="9" t="s">
         <v>49</v>
       </c>
       <c r="L9" s="2" t="n">
@@ -1255,7 +1228,7 @@
       <c r="J10" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="K10" s="9" t="s">
         <v>54</v>
       </c>
       <c r="L10" s="2" t="n">
@@ -1293,7 +1266,7 @@
       <c r="J11" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="K11" s="9" t="s">
+      <c r="K11" s="10" t="s">
         <v>59</v>
       </c>
       <c r="L11" s="2" t="n">
@@ -1331,7 +1304,7 @@
       <c r="J12" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="K12" s="9" t="s">
         <v>64</v>
       </c>
       <c r="L12" s="2" t="n">
@@ -1369,7 +1342,7 @@
       <c r="J13" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="K13" s="2" t="s">
+      <c r="K13" s="9" t="s">
         <v>69</v>
       </c>
       <c r="L13" s="2" t="n">
@@ -1407,7 +1380,7 @@
       <c r="J14" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="K14" s="2" t="s">
+      <c r="K14" s="9" t="s">
         <v>74</v>
       </c>
       <c r="L14" s="2"/>
@@ -1434,7 +1407,7 @@
       <c r="I15" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="K15" s="2" t="s">
+      <c r="K15" s="9" t="s">
         <v>78</v>
       </c>
       <c r="L15" s="2"/>
@@ -1461,7 +1434,7 @@
       <c r="I16" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="K16" s="2" t="s">
+      <c r="K16" s="9" t="s">
         <v>82</v>
       </c>
       <c r="L16" s="2" t="n">
@@ -1499,7 +1472,7 @@
       <c r="J17" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="K17" s="2" t="s">
+      <c r="K17" s="9" t="s">
         <v>87</v>
       </c>
       <c r="L17" s="2"/>
@@ -1535,7 +1508,7 @@
       <c r="J18" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="K18" s="2" t="s">
+      <c r="K18" s="9" t="s">
         <v>92</v>
       </c>
       <c r="L18" s="2"/>
@@ -1571,7 +1544,7 @@
       <c r="J19" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="K19" s="2" t="s">
+      <c r="K19" s="9" t="s">
         <v>97</v>
       </c>
       <c r="L19" s="2"/>
@@ -1607,7 +1580,7 @@
       <c r="J20" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="K20" s="2" t="s">
+      <c r="K20" s="9" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1642,7 +1615,7 @@
       <c r="J21" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="K21" s="2" t="s">
+      <c r="K21" s="9" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1677,7 +1650,7 @@
       <c r="J22" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="K22" s="2" t="s">
+      <c r="K22" s="9" t="s">
         <v>112</v>
       </c>
     </row>
@@ -1712,7 +1685,7 @@
       <c r="J23" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K23" s="2" t="s">
+      <c r="K23" s="9" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1747,7 +1720,7 @@
       <c r="J24" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="K24" s="2" t="s">
+      <c r="K24" s="9" t="s">
         <v>122</v>
       </c>
     </row>
@@ -1773,7 +1746,7 @@
       <c r="I25" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="K25" s="2" t="s">
+      <c r="K25" s="9" t="s">
         <v>126</v>
       </c>
     </row>
@@ -1799,7 +1772,7 @@
       <c r="I26" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="K26" s="2" t="s">
+      <c r="K26" s="9" t="s">
         <v>130</v>
       </c>
     </row>
@@ -1834,7 +1807,7 @@
       <c r="J27" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="K27" s="2" t="s">
+      <c r="K27" s="9" t="s">
         <v>135</v>
       </c>
     </row>
@@ -1869,7 +1842,7 @@
       <c r="J28" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="K28" s="2" t="s">
+      <c r="K28" s="9" t="s">
         <v>140</v>
       </c>
     </row>
@@ -1904,7 +1877,7 @@
       <c r="J29" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="K29" s="2" t="s">
+      <c r="K29" s="9" t="s">
         <v>145</v>
       </c>
     </row>
@@ -1939,7 +1912,7 @@
       <c r="J30" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="K30" s="2" t="s">
+      <c r="K30" s="9" t="s">
         <v>150</v>
       </c>
     </row>
@@ -1974,7 +1947,7 @@
       <c r="J31" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="K31" s="2" t="s">
+      <c r="K31" s="9" t="s">
         <v>155</v>
       </c>
     </row>
@@ -2009,7 +1982,7 @@
       <c r="J32" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="K32" s="2" t="s">
+      <c r="K32" s="9" t="s">
         <v>160</v>
       </c>
     </row>
@@ -2043,7 +2016,7 @@
       <c r="E34" s="3" t="n">
         <v>7500000000</v>
       </c>
-      <c r="F34" s="10" t="n">
+      <c r="F34" s="11" t="n">
         <v>65000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat：updatre areadivide and level
</commit_message>
<xml_diff>
--- a/pet-simulator/Excel/AreaDivide_区域划分表.xlsx
+++ b/pet-simulator/Excel/AreaDivide_区域划分表.xlsx
@@ -343,7 +343,7 @@
     <t xml:space="preserve">-18213|99548|79507</t>
   </si>
   <si>
-    <t xml:space="preserve">-16830.14|-19466.14|101941.13|98405.13|79482.33|80482.33</t>
+    <t xml:space="preserve">-16830.14|102196|-19881|98221.09|79361.22|80258.22</t>
   </si>
   <si>
     <t xml:space="preserve">魔法森林</t>
@@ -370,7 +370,7 @@
     <t xml:space="preserve">1CBF9F29</t>
   </si>
   <si>
-    <t xml:space="preserve">-17138.14|-20689.14|91457.13|88270.13|79225.33|80482.33</t>
+    <t xml:space="preserve">-17138.14|91457.13|-20689.14|88270.13|79225.33|80482.33</t>
   </si>
   <si>
     <t xml:space="preserve">古代遗迹</t>
@@ -385,7 +385,7 @@
     <t xml:space="preserve">12BC0C283CCBEF38</t>
   </si>
   <si>
-    <t xml:space="preserve">-5672.12|-12464.12|120735|113905|65708.25|66832</t>
+    <t xml:space="preserve">-5672.12|120735|-12464.12|113905|65708.25|66832</t>
   </si>
   <si>
     <t xml:space="preserve">樱花庭院</t>
@@ -400,7 +400,7 @@
     <t xml:space="preserve">12BC0C282FD20A42</t>
   </si>
   <si>
-    <t xml:space="preserve">-32149|-37765|99017|89573|78682|80577</t>
+    <t xml:space="preserve">-32149|99017|-37765|89573|78682|80577</t>
   </si>
   <si>
     <t xml:space="preserve">糖果岛</t>
@@ -415,7 +415,7 @@
     <t xml:space="preserve">12BC0C2810A52B8A</t>
   </si>
   <si>
-    <t xml:space="preserve">-24966|-36901|117072|124859|79489|82332</t>
+    <t xml:space="preserve">-24966|117072|-36901|124859|79489|82332</t>
   </si>
   <si>
     <t xml:space="preserve">墓地岛</t>
@@ -430,7 +430,7 @@
     <t xml:space="preserve">12BC0C282374F85D</t>
   </si>
   <si>
-    <t xml:space="preserve">-1264|6759|95949|103610|73002|75359</t>
+    <t xml:space="preserve">-1264|95949|6759|103610|73002|75359</t>
   </si>
   <si>
     <t xml:space="preserve">地狱岛</t>
@@ -445,7 +445,7 @@
     <t xml:space="preserve">12BC0C283F2D14B1</t>
   </si>
   <si>
-    <t xml:space="preserve">-5456|-12251|86882|77509|77334|78540</t>
+    <t xml:space="preserve">-5456|86882|-12251|77509|77334|78540</t>
   </si>
   <si>
     <t xml:space="preserve">天堂岛</t>
@@ -460,7 +460,7 @@
     <t xml:space="preserve">12BC0C283D7AD291</t>
   </si>
   <si>
-    <t xml:space="preserve">-20535|-12992|90706|102852|93142|95702</t>
+    <t xml:space="preserve">-20535|90706|-12992|102852|93142|95702</t>
   </si>
   <si>
     <t xml:space="preserve">大天堂岛</t>
@@ -475,7 +475,7 @@
     <t xml:space="preserve">33EFFD24</t>
   </si>
   <si>
-    <t xml:space="preserve">-18598|-14197|102457|110106|93189|95077</t>
+    <t xml:space="preserve">-18598|102457|-14197|110106|93189|95077</t>
   </si>
   <si>
     <t xml:space="preserve">科技商店</t>
@@ -887,8 +887,8 @@
   </sheetPr>
   <dimension ref="A1:L1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K21" activeCellId="0" sqref="K21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H22" activeCellId="0" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.0859375" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1511,7 +1511,9 @@
       <c r="K18" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="L18" s="2"/>
+      <c r="L18" s="2" t="n">
+        <v>69155</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="n">
@@ -1547,7 +1549,9 @@
       <c r="K19" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="L19" s="2"/>
+      <c r="L19" s="2" t="n">
+        <v>81509</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="n">
@@ -1583,6 +1587,9 @@
       <c r="K20" s="9" t="s">
         <v>102</v>
       </c>
+      <c r="L20" s="1" t="n">
+        <v>82564</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="n">
@@ -1618,6 +1625,9 @@
       <c r="K21" s="9" t="s">
         <v>107</v>
       </c>
+      <c r="L21" s="1" t="n">
+        <v>75515</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="n">
@@ -1653,6 +1663,9 @@
       <c r="K22" s="9" t="s">
         <v>112</v>
       </c>
+      <c r="L22" s="1" t="n">
+        <v>79866</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="n">
@@ -1688,6 +1701,9 @@
       <c r="K23" s="9" t="s">
         <v>117</v>
       </c>
+      <c r="L23" s="1" t="n">
+        <v>94882</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="n">
@@ -1722,6 +1738,9 @@
       </c>
       <c r="K24" s="9" t="s">
         <v>122</v>
+      </c>
+      <c r="L24" s="1" t="n">
+        <v>94882</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
feat：fix world2 wall and treasure location bug
</commit_message>
<xml_diff>
--- a/pet-simulator/Excel/AreaDivide_区域划分表.xlsx
+++ b/pet-simulator/Excel/AreaDivide_区域划分表.xlsx
@@ -472,7 +472,7 @@
     <t xml:space="preserve">-16335|105392|93547</t>
   </si>
   <si>
-    <t xml:space="preserve">33EFFD24</t>
+    <t xml:space="preserve">2B4A0E1C</t>
   </si>
   <si>
     <t xml:space="preserve">-18598|102457|-14197|110106|93189|95077</t>
@@ -601,7 +601,7 @@
     <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * \-??_ ;_ @_ "/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="微软雅黑"/>
@@ -658,6 +658,19 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF000000"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -707,48 +720,56 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -875,10 +896,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J24" activeCellId="0" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.12890625" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1401,6 +1422,7 @@
         <v>78</v>
       </c>
       <c r="L15" s="2"/>
+      <c r="N15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
@@ -1694,6 +1716,7 @@
       <c r="L23" s="1" t="n">
         <v>94882</v>
       </c>
+      <c r="O23" s="10"/>
     </row>
     <row r="24" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="n">
@@ -1723,7 +1746,7 @@
       <c r="I24" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="J24" s="2" t="s">
+      <c r="J24" s="11" t="s">
         <v>121</v>
       </c>
       <c r="K24" s="9" t="s">
@@ -1732,6 +1755,7 @@
       <c r="L24" s="1" t="n">
         <v>94882</v>
       </c>
+      <c r="O24" s="10"/>
     </row>
     <row r="25" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="n">
@@ -2025,7 +2049,7 @@
       <c r="E34" s="3" t="n">
         <v>7500000000</v>
       </c>
-      <c r="F34" s="10" t="n">
+      <c r="F34" s="12" t="n">
         <v>65000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat:update new s2 bug
</commit_message>
<xml_diff>
--- a/pet-simulator/Excel/AreaDivide_区域划分表.xlsx
+++ b/pet-simulator/Excel/AreaDivide_区域划分表.xlsx
@@ -469,7 +469,7 @@
     <t xml:space="preserve">AreaDivide_Name_21</t>
   </si>
   <si>
-    <t xml:space="preserve">-16335|105392|93547</t>
+    <t xml:space="preserve">-16397|104173|93530</t>
   </si>
   <si>
     <t xml:space="preserve">2B4A0E1C</t>
@@ -898,8 +898,8 @@
   </sheetPr>
   <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J24" activeCellId="0" sqref="J24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.12890625" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
fix: minResourceCount in 1009
</commit_message>
<xml_diff>
--- a/pet-simulator/Excel/AreaDivide_区域划分表.xlsx
+++ b/pet-simulator/Excel/AreaDivide_区域划分表.xlsx
@@ -1,31 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\P12GPark\Project\Edit\DragonVerse\pet-simulator\Excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F46423E-AD4B-474E-8F12-9BB4B3C63DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="20640" windowHeight="14184" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="163">
   <si>
     <t>int</t>
   </si>
@@ -76,6 +65,9 @@
   </si>
   <si>
     <t>dropItemPlatform</t>
+  </si>
+  <si>
+    <t>minResourceCount</t>
   </si>
   <si>
     <t>区域说明（策划看）</t>
@@ -85,7 +77,6 @@
       <rPr>
         <sz val="10.5"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
         <charset val="134"/>
       </rPr>
       <t>是否需要解锁</t>
@@ -94,7 +85,6 @@
       <rPr>
         <sz val="10.5"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
         <charset val="1"/>
       </rPr>
       <t>1=</t>
@@ -103,7 +93,6 @@
       <rPr>
         <sz val="10.5"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
         <charset val="134"/>
       </rPr>
       <t>需要；</t>
@@ -112,7 +101,6 @@
       <rPr>
         <sz val="10.5"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
         <charset val="1"/>
       </rPr>
       <t>0=</t>
@@ -121,7 +109,6 @@
       <rPr>
         <sz val="10.5"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
         <charset val="134"/>
       </rPr>
       <t>不需要</t>
@@ -132,7 +119,6 @@
       <rPr>
         <sz val="10.5"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
         <charset val="134"/>
       </rPr>
       <t>货币种类（货币表</t>
@@ -141,7 +127,6 @@
       <rPr>
         <sz val="10.5"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
         <charset val="1"/>
       </rPr>
       <t>id</t>
@@ -150,7 +135,6 @@
       <rPr>
         <sz val="10.5"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
         <charset val="134"/>
       </rPr>
       <t>）</t>
@@ -176,7 +160,6 @@
       <rPr>
         <sz val="10.5"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
         <charset val="134"/>
       </rPr>
       <t>区域划分点坐标数组</t>
@@ -185,7 +168,6 @@
       <rPr>
         <sz val="10.5"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
         <charset val="1"/>
       </rPr>
       <t>Xmin|Ymin|Xmax|Ymax</t>
@@ -195,6 +177,9 @@
     <t>掉落物平台高度</t>
   </si>
   <si>
+    <t>区域内资源刷新数量下限 默认100</t>
+  </si>
+  <si>
     <t>Language</t>
   </si>
   <si>
@@ -600,70 +585,211 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="5">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * \-??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="28">
     <font>
       <sz val="10"/>
       <name val="微软雅黑"/>
-      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="微软雅黑"/>
-      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="10.5"/>
       <name val="Calibri"/>
-      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="10.5"/>
       <name val="微软雅黑"/>
-      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="9.75"/>
       <name val="Calibri"/>
-      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="10.5"/>
       <color rgb="FF000000"/>
       <name val="微软雅黑"/>
-      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="10.5"/>
       <name val="Calibri"/>
-      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="微软雅黑"/>
-      <family val="2"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="DejaVu Sans"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="DejaVu Sans"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="DejaVu Sans"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="DejaVu Sans"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="DejaVu Sans"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="DejaVu Sans"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="DejaVu Sans"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="DejaVu Sans"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="DejaVu Sans"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="DejaVu Sans"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="DejaVu Sans"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="DejaVu Sans"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="DejaVu Sans"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="DejaVu Sans"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="DejaVu Sans"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="DejaVu Sans"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="DejaVu Sans"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="DejaVu Sans"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="DejaVu Sans"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="DejaVu Sans"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -676,8 +802,194 @@
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -685,9 +997,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -707,24 +1261,68 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="176" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -783,7 +1381,7 @@
         <a:cs typeface="DejaVu Sans"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme>
+    <a:fmtScheme name="">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -834,37 +1432,38 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.125" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="12.1287878787879" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.87878787878788" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6287878787879" style="1" customWidth="1"/>
     <col min="3" max="3" width="15.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="13" style="1" customWidth="1"/>
     <col min="5" max="5" width="15.5" style="1" customWidth="1"/>
     <col min="6" max="6" width="20.75" style="1" customWidth="1"/>
     <col min="7" max="7" width="11.25" style="1" customWidth="1"/>
-    <col min="8" max="8" width="22.375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="22.3787878787879" style="1" customWidth="1"/>
     <col min="9" max="9" width="20.75" style="1" customWidth="1"/>
-    <col min="10" max="10" width="25.875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="25.8787878787879" style="1" customWidth="1"/>
     <col min="11" max="11" width="63" style="1" customWidth="1"/>
-    <col min="12" max="12" width="6.875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="7.75" style="1" customWidth="1"/>
-    <col min="14" max="19" width="6.875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="6.87878787878788" style="1" customWidth="1"/>
+    <col min="13" max="13" width="32.1818181818182" style="1" customWidth="1"/>
+    <col min="14" max="14" width="12.0909090909091" style="1" customWidth="1"/>
+    <col min="15" max="19" width="6.87878787878788" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" ht="18" customHeight="1" spans="1:13">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -901,8 +1500,11 @@
       <c r="L1" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="M1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" ht="18" customHeight="1" spans="1:13">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -939,55 +1541,61 @@
       <c r="L2" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="M2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" ht="33" customHeight="1" spans="1:13">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+        <v>27</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" ht="18" customHeight="1" spans="8:12">
       <c r="H4" s="7" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" ht="18" customHeight="1" spans="1:12">
       <c r="A5" s="2">
         <v>1001</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C5" s="2">
         <v>0</v>
@@ -999,22 +1607,22 @@
         <v>177826</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K5" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" ht="18" customHeight="1" spans="1:12">
       <c r="A6" s="2">
         <v>1002</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C6" s="2">
         <v>0</v>
@@ -1026,24 +1634,24 @@
         <v>174840</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="K6" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>37</v>
       </c>
       <c r="L6" s="2">
         <v>1000</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" ht="18" customHeight="1" spans="1:12">
       <c r="A7" s="2">
         <v>1003</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C7" s="2">
         <v>1</v>
@@ -1061,27 +1669,27 @@
         <v>144238</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="K7" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>42</v>
       </c>
       <c r="L7" s="2">
         <v>1000</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" ht="18" customHeight="1" spans="1:12">
       <c r="A8" s="2">
         <v>1004</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C8" s="2">
         <v>1</v>
@@ -1099,27 +1707,27 @@
         <v>180217</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="K8" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="L8" s="2">
         <v>1000</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" ht="18" customHeight="1" spans="1:12">
       <c r="A9" s="2">
         <v>1005</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C9" s="2">
         <v>1</v>
@@ -1137,27 +1745,27 @@
         <v>180218</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="J9" s="2">
         <v>32519069</v>
       </c>
-      <c r="K9" s="9" t="s">
-        <v>49</v>
+      <c r="K9" s="10" t="s">
+        <v>51</v>
       </c>
       <c r="L9" s="2">
         <v>1000</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" ht="18" customHeight="1" spans="1:12">
       <c r="A10" s="2">
         <v>1006</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C10" s="2">
         <v>1</v>
@@ -1175,27 +1783,27 @@
         <v>174840</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="K10" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>56</v>
       </c>
       <c r="L10" s="2">
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" ht="18" customHeight="1" spans="1:12">
       <c r="A11" s="2">
         <v>1007</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C11" s="2">
         <v>1</v>
@@ -1213,27 +1821,27 @@
         <v>174840</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="K11" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
+      </c>
+      <c r="K11" s="10" t="s">
+        <v>61</v>
       </c>
       <c r="L11" s="2">
         <v>1000</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" ht="18" customHeight="1" spans="1:12">
       <c r="A12" s="2">
         <v>1008</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C12" s="2">
         <v>1</v>
@@ -1251,27 +1859,27 @@
         <v>174840</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="K12" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
+      </c>
+      <c r="K12" s="10" t="s">
+        <v>66</v>
       </c>
       <c r="L12" s="2">
         <v>1000</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" ht="18" customHeight="1" spans="1:13">
       <c r="A13" s="2">
         <v>1009</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C13" s="2">
         <v>1</v>
@@ -1289,27 +1897,30 @@
         <v>174833</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="K13" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
+      </c>
+      <c r="K13" s="10" t="s">
+        <v>71</v>
       </c>
       <c r="L13" s="2">
         <v>1000</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="M13" s="1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="14" ht="18" customHeight="1" spans="1:12">
       <c r="A14" s="2">
         <v>1010</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C14" s="2">
         <v>1</v>
@@ -1327,25 +1938,25 @@
         <v>174840</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="K14" s="9" t="s">
-        <v>74</v>
+        <v>75</v>
+      </c>
+      <c r="K14" s="10" t="s">
+        <v>76</v>
       </c>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" ht="18" customHeight="1" spans="1:14">
       <c r="A15" s="2">
         <v>2001</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C15" s="2">
         <v>1</v>
@@ -1357,23 +1968,23 @@
         <v>177826</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="K15" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
+      </c>
+      <c r="K15" s="10" t="s">
+        <v>80</v>
       </c>
       <c r="L15" s="2"/>
-      <c r="N15" s="10"/>
-    </row>
-    <row r="16" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N15" s="11"/>
+    </row>
+    <row r="16" ht="18" customHeight="1" spans="1:12">
       <c r="A16" s="2">
         <v>2002</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C16" s="2">
         <v>1</v>
@@ -1385,24 +1996,24 @@
         <v>180217</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="K16" s="9" t="s">
-        <v>82</v>
+        <v>83</v>
+      </c>
+      <c r="K16" s="10" t="s">
+        <v>84</v>
       </c>
       <c r="L16" s="2">
         <v>81000</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" ht="18" customHeight="1" spans="1:12">
       <c r="A17" s="2">
         <v>2003</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C17" s="2">
         <v>1</v>
@@ -1420,25 +2031,25 @@
         <v>174840</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="K17" s="9" t="s">
-        <v>87</v>
+        <v>88</v>
+      </c>
+      <c r="K17" s="10" t="s">
+        <v>89</v>
       </c>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" ht="18" customHeight="1" spans="1:12">
       <c r="A18" s="2">
         <v>2004</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C18" s="2">
         <v>1</v>
@@ -1456,27 +2067,27 @@
         <v>174840</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="K18" s="9" t="s">
-        <v>92</v>
+        <v>93</v>
+      </c>
+      <c r="K18" s="10" t="s">
+        <v>94</v>
       </c>
       <c r="L18" s="2">
         <v>69155</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" ht="18" customHeight="1" spans="1:12">
       <c r="A19" s="2">
         <v>2005</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C19" s="2">
         <v>1</v>
@@ -1494,27 +2105,27 @@
         <v>174840</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="K19" s="9" t="s">
-        <v>97</v>
+        <v>98</v>
+      </c>
+      <c r="K19" s="10" t="s">
+        <v>99</v>
       </c>
       <c r="L19" s="2">
         <v>81509</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" ht="18" customHeight="1" spans="1:12">
       <c r="A20" s="2">
         <v>2006</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C20" s="2">
         <v>1</v>
@@ -1532,27 +2143,27 @@
         <v>174840</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="K20" s="9" t="s">
-        <v>102</v>
+        <v>103</v>
+      </c>
+      <c r="K20" s="10" t="s">
+        <v>104</v>
       </c>
       <c r="L20" s="1">
         <v>82564</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" ht="18" customHeight="1" spans="1:12">
       <c r="A21" s="2">
         <v>2007</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C21" s="2">
         <v>1</v>
@@ -1570,27 +2181,27 @@
         <v>174840</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="K21" s="9" t="s">
-        <v>107</v>
+        <v>108</v>
+      </c>
+      <c r="K21" s="10" t="s">
+        <v>109</v>
       </c>
       <c r="L21" s="1">
         <v>75515</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" ht="18" customHeight="1" spans="1:12">
       <c r="A22" s="2">
         <v>2008</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C22" s="2">
         <v>1</v>
@@ -1608,27 +2219,27 @@
         <v>174840</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="K22" s="9" t="s">
-        <v>112</v>
+        <v>113</v>
+      </c>
+      <c r="K22" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="L22" s="1">
         <v>79866</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" ht="18" customHeight="1" spans="1:15">
       <c r="A23" s="2">
         <v>2009</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C23" s="2">
         <v>1</v>
@@ -1646,28 +2257,28 @@
         <v>174840</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="K23" s="9" t="s">
-        <v>117</v>
+        <v>118</v>
+      </c>
+      <c r="K23" s="10" t="s">
+        <v>119</v>
       </c>
       <c r="L23" s="1">
         <v>94882</v>
       </c>
-      <c r="O23" s="10"/>
-    </row>
-    <row r="24" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O23" s="11"/>
+    </row>
+    <row r="24" ht="18" customHeight="1" spans="1:15">
       <c r="A24" s="2">
         <v>2010</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C24" s="2">
         <v>1</v>
@@ -1685,28 +2296,28 @@
         <v>174840</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="J24" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="K24" s="9" t="s">
         <v>122</v>
+      </c>
+      <c r="J24" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="K24" s="10" t="s">
+        <v>124</v>
       </c>
       <c r="L24" s="1">
         <v>94882</v>
       </c>
-      <c r="O24" s="10"/>
-    </row>
-    <row r="25" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O24" s="11"/>
+    </row>
+    <row r="25" ht="18" customHeight="1" spans="1:11">
       <c r="A25" s="2">
         <v>3001</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C25" s="2">
         <v>1</v>
@@ -1718,21 +2329,21 @@
         <v>177826</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="K25" s="9" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+        <v>127</v>
+      </c>
+      <c r="K25" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="26" ht="18" customHeight="1" spans="1:11">
       <c r="A26" s="2">
         <v>3002</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C26" s="2">
         <v>1</v>
@@ -1744,21 +2355,21 @@
         <v>174840</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="K26" s="9" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+        <v>131</v>
+      </c>
+      <c r="K26" s="10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="27" ht="18" customHeight="1" spans="1:11">
       <c r="A27" s="2">
         <v>3003</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C27" s="2">
         <v>1</v>
@@ -1776,24 +2387,24 @@
         <v>174840</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="K27" s="9" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+        <v>136</v>
+      </c>
+      <c r="K27" s="10" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="28" ht="18" customHeight="1" spans="1:11">
       <c r="A28" s="2">
         <v>3004</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C28" s="2">
         <v>1</v>
@@ -1811,24 +2422,24 @@
         <v>174840</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="K28" s="9" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+        <v>141</v>
+      </c>
+      <c r="K28" s="10" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="29" ht="18" customHeight="1" spans="1:11">
       <c r="A29" s="2">
         <v>3005</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C29" s="2">
         <v>1</v>
@@ -1846,24 +2457,24 @@
         <v>174840</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="K29" s="9" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+        <v>146</v>
+      </c>
+      <c r="K29" s="10" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="30" ht="18" customHeight="1" spans="1:11">
       <c r="A30" s="2">
         <v>3006</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C30" s="2">
         <v>1</v>
@@ -1881,24 +2492,24 @@
         <v>174840</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="K30" s="9" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+        <v>151</v>
+      </c>
+      <c r="K30" s="10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="31" ht="18" customHeight="1" spans="1:11">
       <c r="A31" s="2">
         <v>3007</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C31" s="2">
         <v>1</v>
@@ -1916,24 +2527,24 @@
         <v>174840</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="K31" s="9" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+      <c r="K31" s="10" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="32" ht="18" customHeight="1" spans="1:11">
       <c r="A32" s="2">
         <v>3008</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C32" s="2">
         <v>1</v>
@@ -1951,19 +2562,19 @@
         <v>174840</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="K32" s="9" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+        <v>161</v>
+      </c>
+      <c r="K32" s="10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="33" ht="18" customHeight="1" spans="1:6">
       <c r="A33" s="2">
         <v>3009</v>
       </c>
@@ -1980,7 +2591,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" ht="18" customHeight="1" spans="1:6">
       <c r="A34" s="2">
         <v>3010</v>
       </c>
@@ -1993,13 +2604,13 @@
       <c r="E34" s="3">
         <v>7500000000</v>
       </c>
-      <c r="F34" s="12">
+      <c r="F34" s="9">
         <v>65000</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>